<commit_message>
#phuc.nguyen fix button search in index
</commit_message>
<xml_diff>
--- a/docs/yeuCau.xlsx
+++ b/docs/yeuCau.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\real_estate\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\real_estate\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D66A67-E6CD-43ED-A436-E26E0B8CC159}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CT258 pt tmdt" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CT258 pt tmdt'!$A$1:$C$23</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="75">
   <si>
     <t>Max-5sv</t>
   </si>
@@ -271,44 +270,17 @@
     <t>Báo cáo cho nhóm (tại phòng học hoặc bộ môn)</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>dễ</t>
-  </si>
-  <si>
-    <t>1/2</t>
-  </si>
-  <si>
-    <t>trung bình</t>
-  </si>
-  <si>
-    <t>khó</t>
-  </si>
-  <si>
-    <t>Phụng</t>
-  </si>
-  <si>
-    <t>Phúc</t>
-  </si>
-  <si>
-    <t>Thắm/Tâm</t>
-  </si>
-  <si>
-    <t>Nghĩa</t>
+    <t>ü</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -375,20 +347,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Wingdings 2"/>
-      <family val="1"/>
-      <charset val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -397,8 +355,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,24 +383,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF66"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF66FF66"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -465,30 +417,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -513,22 +445,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -549,57 +470,40 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -817,252 +721,206 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="105.125" customWidth="1"/>
-    <col min="3" max="26" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="105.09765625" customWidth="1"/>
+    <col min="3" max="24" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="36"/>
       <c r="C1" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="25">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="53"/>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A3" s="29">
+      <c r="D2" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="23"/>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A4" s="29">
+    </row>
+    <row r="4" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A4" s="23">
         <v>3</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" s="23"/>
-    </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A5" s="29">
+      <c r="D4" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A5" s="23">
         <v>4</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" s="23"/>
-    </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="29">
+      <c r="D5" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A6" s="23">
         <v>5</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="23"/>
-    </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="29">
+      <c r="D6" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A7" s="23">
         <v>6</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="23"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A8" s="29">
+    </row>
+    <row r="8" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A8" s="23">
         <v>7</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" s="53"/>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="29">
+      <c r="D8" s="38"/>
+    </row>
+    <row r="9" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A9" s="23">
         <v>8</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" s="53"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="29">
+      <c r="D9" s="38"/>
+    </row>
+    <row r="10" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A10" s="23">
         <v>9</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="53"/>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="29">
+      <c r="D10" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A11" s="23">
         <v>10</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F11" s="23"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="29">
+      <c r="D11" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A12" s="23">
         <v>11</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" s="23"/>
-    </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="29">
+      <c r="D12" s="38"/>
+    </row>
+    <row r="13" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A13" s="23">
         <v>12</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="23"/>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="38">
+    </row>
+    <row r="14" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A14" s="26">
         <v>13</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="37" t="s">
         <v>74</v>
       </c>
       <c r="E14" s="13"/>
-      <c r="F14" s="54"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
@@ -1081,191 +939,171 @@
       <c r="V14" s="13"/>
       <c r="W14" s="13"/>
       <c r="X14" s="13"/>
-      <c r="Y14" s="13"/>
-      <c r="Z14" s="13"/>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="25">
+    </row>
+    <row r="15" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A15" s="20">
         <v>14</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="23"/>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A16" s="29">
+    </row>
+    <row r="16" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A16" s="23">
         <v>15</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" s="23"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A17" s="46">
+      <c r="D16" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A17" s="31">
         <v>16</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="23"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A18" s="46">
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A18" s="31">
         <v>17</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="23"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A19" s="46">
+      <c r="D18" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A19" s="31">
         <v>18</v>
       </c>
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" s="23"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A20" s="46">
+      <c r="D19" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A20" s="31">
         <v>19</v>
       </c>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="F20" s="23"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A21" s="46">
+      <c r="D20" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A21" s="31">
         <v>20</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="38"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A22" s="31">
+        <v>21</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="23"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A22" s="46">
-        <v>21</v>
-      </c>
-      <c r="B22" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="31" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A23" s="31">
+        <v>22</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="49" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A23" s="46">
-        <v>22</v>
-      </c>
-      <c r="B23" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="31" t="s">
+      <c r="D23" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A24" s="26">
+        <v>23</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="D24" s="37" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A24" s="38">
-        <v>23</v>
-      </c>
-      <c r="B24" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="52" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1">
       <c r="A25" s="15"/>
       <c r="B25" s="16"/>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1">
       <c r="A26" s="15"/>
       <c r="B26" s="16"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1">
       <c r="B27" s="17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1">
       <c r="B28" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1">
       <c r="C30" s="13"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1">
+    <row r="31" spans="1:4" ht="15.75" customHeight="1">
       <c r="C31" s="13"/>
     </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1">
+    <row r="32" spans="1:4" ht="15.75" customHeight="1">
       <c r="C32" s="13"/>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1">
@@ -2369,18 +2207,18 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:C23" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C23"/>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <phoneticPr fontId="15" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2388,9 +2226,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="35.75" customWidth="1"/>
+    <col min="2" max="2" width="35.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2514,25 +2352,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="C5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="C6" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="C11" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C5" r:id="rId2"/>
+    <hyperlink ref="C6" r:id="rId3"/>
+    <hyperlink ref="C11" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>

</xml_diff>